<commit_message>
Add Stat Grad 10.12
</commit_message>
<xml_diff>
--- a/Solutions_1921_Excel/1921.xlsx
+++ b/Solutions_1921_Excel/1921.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hem12\Documents\Документы Миша\Школьные предметы\ЕГЭ информатика\Solutions\PrepareForEGE_MishaPolykovsky\Solutions_1921_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D91C85-2257-4E2B-A0BB-7B07174E657D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF6C414-83F4-4A3A-8647-2FCE45F39267}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>3 14</t>
   </si>
@@ -30,12 +30,27 @@
   <si>
     <t>28 30</t>
   </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>11 32</t>
+  </si>
+  <si>
+    <t>22 42</t>
+  </si>
+  <si>
+    <t>12 11</t>
+  </si>
+  <si>
+    <t>12 39</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,8 +82,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,12 +136,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,7 +184,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1"/>
@@ -177,7 +194,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -185,6 +201,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Вывод" xfId="1" builtinId="21"/>
@@ -193,6 +211,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCF3131"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -714,13 +737,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -738,6 +761,165 @@
         <a:xfrm>
           <a:off x="4467225" y="22926675"/>
           <a:ext cx="38100" cy="2333625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Прямая со стрелкой 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4062278-2515-4351-8D4D-87B5174CC97E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3448050" y="20288250"/>
+          <a:ext cx="2962276" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Прямая со стрелкой 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C282BF1-CBF7-44B6-A422-CB01DBDA0915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762250" y="18773775"/>
+          <a:ext cx="3724275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Прямая со стрелкой 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{866951BD-012E-4988-9A0F-08FB4021A3A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="23917275"/>
+          <a:ext cx="2476500" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1064,10 +1246,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE76F85B-B0D9-9145-A11D-59C0FC73726D}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="C4:V134"/>
+  <dimension ref="C4:V147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O129" sqref="O129"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="T119" sqref="T119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2132,419 +2314,485 @@
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="98" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C98" s="10">
-        <v>47</v>
+    <row r="98" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C98" s="9">
+        <v>41</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1">
-        <v>1</v>
-      </c>
-      <c r="F98" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H98" s="1">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I98" s="1">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J98" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K98" s="1">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="L98" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M98" s="1">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N98" s="1">
-        <v>10</v>
-      </c>
-      <c r="O98" s="1">
-        <v>11</v>
-      </c>
-      <c r="P98" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="3:18" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="P98">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="7"/>
-      <c r="J99" s="9"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="7"/>
-      <c r="N99" s="5"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="2"/>
-      <c r="R99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C106" s="10">
-        <v>49</v>
+      <c r="E99" s="5"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="P99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C106" s="17">
+        <v>47</v>
       </c>
       <c r="D106" s="1"/>
       <c r="E106" s="1">
+        <v>11</v>
+      </c>
+      <c r="F106" s="1">
+        <v>12</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H106" s="1">
+        <v>32</v>
+      </c>
+      <c r="I106" s="1">
+        <v>33</v>
+      </c>
+      <c r="J106" s="1">
+        <v>34</v>
+      </c>
+      <c r="K106" s="1">
+        <v>35</v>
+      </c>
+      <c r="M106" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="107" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="2"/>
+      <c r="G107" s="1"/>
+      <c r="H107" s="7"/>
+      <c r="I107" s="5"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="2"/>
+      <c r="M107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M108" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C114" s="9">
+        <v>49</v>
+      </c>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1">
+        <v>20</v>
+      </c>
+      <c r="F114" s="1">
+        <v>21</v>
+      </c>
+      <c r="G114" s="1">
+        <v>22</v>
+      </c>
+      <c r="H114" s="1">
+        <v>23</v>
+      </c>
+      <c r="I114" s="1">
+        <v>24</v>
+      </c>
+      <c r="K114" s="1">
+        <v>42</v>
+      </c>
+      <c r="M114">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C115" s="1">
         <v>10</v>
       </c>
-      <c r="F106" s="1">
+      <c r="D115" s="1"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="7"/>
+      <c r="K115" s="5"/>
+      <c r="M115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C116" s="1">
+        <v>9</v>
+      </c>
+      <c r="D116" s="1"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="3"/>
+      <c r="I116" s="5"/>
+      <c r="M116">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C117" s="1">
+        <v>8</v>
+      </c>
+      <c r="D117" s="1"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="3"/>
+    </row>
+    <row r="118" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C118" s="1">
+        <v>7</v>
+      </c>
+      <c r="D118" s="1"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="125" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C125" s="1">
+        <v>48</v>
+      </c>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1">
+        <v>7</v>
+      </c>
+      <c r="G125" s="1">
+        <v>12</v>
+      </c>
+      <c r="H125" s="1">
+        <v>13</v>
+      </c>
+      <c r="I125" s="1">
+        <v>14</v>
+      </c>
+      <c r="J125" s="1">
+        <v>15</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L125" s="1">
+        <v>39</v>
+      </c>
+      <c r="M125" s="1">
+        <v>40</v>
+      </c>
+      <c r="N125" s="1">
+        <v>41</v>
+      </c>
+      <c r="O125" s="1">
+        <v>42</v>
+      </c>
+      <c r="Q125">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="5"/>
+      <c r="G126" s="7"/>
+      <c r="H126" s="5"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="2"/>
+      <c r="K126" s="1"/>
+      <c r="L126" s="7"/>
+      <c r="M126" s="5"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="2"/>
+      <c r="Q126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q127" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C133" s="10">
+        <v>57</v>
+      </c>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10">
+        <v>25</v>
+      </c>
+      <c r="F133" s="10">
+        <v>26</v>
+      </c>
+      <c r="G133" s="10">
+        <v>27</v>
+      </c>
+      <c r="H133" s="10">
+        <v>28</v>
+      </c>
+      <c r="I133" s="10">
+        <v>29</v>
+      </c>
+      <c r="J133" s="10">
+        <v>30</v>
+      </c>
+      <c r="K133" s="10">
+        <v>31</v>
+      </c>
+      <c r="L133" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="134" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C134" s="10">
+        <v>4</v>
+      </c>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="11"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="11"/>
+      <c r="J134" s="12"/>
+      <c r="K134" s="13"/>
+      <c r="L134" s="14"/>
+      <c r="N134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C135" s="10">
+        <v>5</v>
+      </c>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
+      <c r="H135" s="10"/>
+      <c r="I135" s="10"/>
+      <c r="J135" s="10"/>
+      <c r="K135" s="14"/>
+      <c r="L135" s="14"/>
+      <c r="N135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C136" s="10">
+        <v>6</v>
+      </c>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+      <c r="G136" s="10"/>
+      <c r="H136" s="10"/>
+      <c r="I136" s="10"/>
+      <c r="J136" s="10"/>
+      <c r="K136" s="14"/>
+      <c r="L136" s="14"/>
+      <c r="N136">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="137" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C137" s="10">
+        <v>7</v>
+      </c>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="11"/>
+      <c r="J137" s="12"/>
+      <c r="K137" s="14"/>
+      <c r="L137" s="14"/>
+    </row>
+    <row r="138" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C138" s="10">
+        <v>8</v>
+      </c>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+      <c r="G138" s="10"/>
+      <c r="H138" s="10"/>
+      <c r="I138" s="12"/>
+      <c r="J138" s="13"/>
+      <c r="K138" s="14"/>
+      <c r="L138" s="14"/>
+    </row>
+    <row r="139" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C139" s="10">
+        <v>9</v>
+      </c>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
+      <c r="H139" s="10"/>
+      <c r="I139" s="15"/>
+      <c r="J139" s="14"/>
+      <c r="K139" s="14"/>
+      <c r="L139" s="14"/>
+    </row>
+    <row r="140" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C140" s="10">
+        <v>10</v>
+      </c>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
+      <c r="H140" s="10"/>
+      <c r="I140" s="15"/>
+      <c r="J140" s="14"/>
+      <c r="K140" s="14"/>
+      <c r="L140" s="14"/>
+    </row>
+    <row r="141" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C141" s="10">
         <v>11</v>
       </c>
-      <c r="G106" s="1">
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="11"/>
+      <c r="I141" s="12"/>
+      <c r="J141" s="14"/>
+      <c r="K141" s="14"/>
+      <c r="L141" s="14"/>
+    </row>
+    <row r="142" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C142" s="10">
         <v>12</v>
       </c>
-      <c r="H106" s="1">
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
+      <c r="H142" s="12"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="14"/>
+      <c r="K142" s="14"/>
+      <c r="L142" s="14"/>
+    </row>
+    <row r="143" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C143" s="10">
         <v>13</v>
       </c>
-      <c r="I106" s="1">
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="14"/>
+      <c r="J143" s="14"/>
+      <c r="K143" s="14"/>
+      <c r="L143" s="14"/>
+    </row>
+    <row r="144" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C144" s="10">
         <v>14</v>
       </c>
-      <c r="J106" s="1">
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+      <c r="G144" s="10"/>
+      <c r="H144" s="10"/>
+      <c r="I144" s="14"/>
+      <c r="J144" s="14"/>
+      <c r="K144" s="14"/>
+      <c r="L144" s="14"/>
+    </row>
+    <row r="145" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C145" s="10">
         <v>15</v>
       </c>
-      <c r="K106" s="1">
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+      <c r="G145" s="11"/>
+      <c r="H145" s="12"/>
+      <c r="I145" s="14"/>
+      <c r="J145" s="14"/>
+      <c r="K145" s="14"/>
+      <c r="L145" s="14"/>
+    </row>
+    <row r="146" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C146" s="10">
         <v>16</v>
       </c>
-    </row>
-    <row r="107" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C107" s="1">
-        <v>4</v>
-      </c>
-      <c r="D107" s="1"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-    </row>
-    <row r="108" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C108" s="1">
-        <v>5</v>
-      </c>
-      <c r="D108" s="1"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="1"/>
-    </row>
-    <row r="109" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C109" s="1">
-        <v>6</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
-    </row>
-    <row r="110" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C110" s="1">
-        <v>7</v>
-      </c>
-      <c r="D110" s="1"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
-    </row>
-    <row r="111" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C111" s="1">
-        <v>8</v>
-      </c>
-      <c r="D111" s="1"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="1"/>
-      <c r="I111" s="1"/>
-      <c r="J111" s="1"/>
-      <c r="K111" s="1"/>
-    </row>
-    <row r="112" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C112" s="1">
-        <v>9</v>
-      </c>
-      <c r="D112" s="1"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="1"/>
-      <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
-      <c r="J112" s="1"/>
-      <c r="K112" s="1"/>
-    </row>
-    <row r="113" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C113" s="1">
-        <v>10</v>
-      </c>
-      <c r="D113" s="1"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="1"/>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1"/>
-      <c r="I113" s="1"/>
-      <c r="J113" s="1"/>
-      <c r="K113" s="1"/>
-    </row>
-    <row r="120" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C120" s="11">
-        <v>57</v>
-      </c>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11">
-        <v>25</v>
-      </c>
-      <c r="F120" s="11">
-        <v>26</v>
-      </c>
-      <c r="G120" s="11">
-        <v>27</v>
-      </c>
-      <c r="H120" s="11">
-        <v>28</v>
-      </c>
-      <c r="I120" s="11">
-        <v>29</v>
-      </c>
-      <c r="J120" s="11">
-        <v>30</v>
-      </c>
-      <c r="K120" s="11">
-        <v>31</v>
-      </c>
-      <c r="L120" s="11">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="121" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C121" s="11">
-        <v>4</v>
-      </c>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
-      <c r="F121" s="11"/>
-      <c r="G121" s="12"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="12"/>
-      <c r="J121" s="13"/>
-      <c r="K121" s="14"/>
-      <c r="L121" s="15"/>
-      <c r="N121">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C122" s="11">
-        <v>5</v>
-      </c>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
-      <c r="H122" s="11"/>
-      <c r="I122" s="11"/>
-      <c r="J122" s="11"/>
-      <c r="K122" s="15"/>
-      <c r="L122" s="15"/>
-      <c r="N122" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="123" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C123" s="11">
-        <v>6</v>
-      </c>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
-      <c r="H123" s="11"/>
-      <c r="I123" s="11"/>
-      <c r="J123" s="11"/>
-      <c r="K123" s="15"/>
-      <c r="L123" s="15"/>
-      <c r="N123">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="124" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C124" s="11">
-        <v>7</v>
-      </c>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
-      <c r="H124" s="11"/>
-      <c r="I124" s="12"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="15"/>
-      <c r="L124" s="15"/>
-    </row>
-    <row r="125" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C125" s="11">
-        <v>8</v>
-      </c>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
-      <c r="H125" s="11"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="14"/>
-      <c r="K125" s="15"/>
-      <c r="L125" s="15"/>
-    </row>
-    <row r="126" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C126" s="11">
-        <v>9</v>
-      </c>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
-      <c r="F126" s="11"/>
-      <c r="G126" s="11"/>
-      <c r="H126" s="11"/>
-      <c r="I126" s="16"/>
-      <c r="J126" s="15"/>
-      <c r="K126" s="15"/>
-      <c r="L126" s="15"/>
-    </row>
-    <row r="127" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C127" s="11">
-        <v>10</v>
-      </c>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
-      <c r="F127" s="11"/>
-      <c r="G127" s="11"/>
-      <c r="H127" s="11"/>
-      <c r="I127" s="16"/>
-      <c r="J127" s="15"/>
-      <c r="K127" s="15"/>
-      <c r="L127" s="15"/>
-    </row>
-    <row r="128" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C128" s="11">
-        <v>11</v>
-      </c>
-      <c r="D128" s="11"/>
-      <c r="E128" s="11"/>
-      <c r="F128" s="11"/>
-      <c r="G128" s="11"/>
-      <c r="H128" s="12"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="15"/>
-      <c r="K128" s="15"/>
-      <c r="L128" s="15"/>
-    </row>
-    <row r="129" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C129" s="11">
-        <v>12</v>
-      </c>
-      <c r="D129" s="11"/>
-      <c r="E129" s="11"/>
-      <c r="F129" s="11"/>
-      <c r="G129" s="11"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="14"/>
-      <c r="J129" s="15"/>
-      <c r="K129" s="15"/>
-      <c r="L129" s="15"/>
-    </row>
-    <row r="130" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C130" s="11">
-        <v>13</v>
-      </c>
-      <c r="D130" s="11"/>
-      <c r="E130" s="11"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="11"/>
-      <c r="H130" s="11"/>
-      <c r="I130" s="15"/>
-      <c r="J130" s="15"/>
-      <c r="K130" s="15"/>
-      <c r="L130" s="15"/>
-    </row>
-    <row r="131" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C131" s="11">
-        <v>14</v>
-      </c>
-      <c r="D131" s="11"/>
-      <c r="E131" s="11"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="11"/>
-      <c r="H131" s="11"/>
-      <c r="I131" s="15"/>
-      <c r="J131" s="15"/>
-      <c r="K131" s="15"/>
-      <c r="L131" s="15"/>
-    </row>
-    <row r="132" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C132" s="11">
-        <v>15</v>
-      </c>
-      <c r="D132" s="11"/>
-      <c r="E132" s="11"/>
-      <c r="F132" s="11"/>
-      <c r="G132" s="12"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="15"/>
-      <c r="J132" s="15"/>
-      <c r="K132" s="15"/>
-      <c r="L132" s="15"/>
-    </row>
-    <row r="133" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C133" s="11">
-        <v>16</v>
-      </c>
-      <c r="D133" s="11"/>
-      <c r="E133" s="11"/>
-      <c r="F133" s="11"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="14"/>
-      <c r="I133" s="15"/>
-      <c r="J133" s="15"/>
-      <c r="K133" s="15"/>
-      <c r="L133" s="15"/>
-    </row>
-    <row r="134" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C134" s="11">
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+      <c r="G146" s="12"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="14"/>
+      <c r="J146" s="14"/>
+      <c r="K146" s="14"/>
+      <c r="L146" s="14"/>
+    </row>
+    <row r="147" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C147" s="10">
         <v>17</v>
       </c>
-      <c r="D134" s="11"/>
-      <c r="E134" s="11"/>
-      <c r="F134" s="11"/>
-      <c r="G134" s="11"/>
-      <c r="H134" s="15"/>
-      <c r="I134" s="15"/>
-      <c r="J134" s="15"/>
-      <c r="K134" s="15"/>
-      <c r="L134" s="15"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="14"/>
+      <c r="I147" s="14"/>
+      <c r="J147" s="14"/>
+      <c r="K147" s="14"/>
+      <c r="L147" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>